<commit_message>
Updating the initial condition equations
</commit_message>
<xml_diff>
--- a/code-Spring2025/NestedBinaryData.xlsx
+++ b/code-Spring2025/NestedBinaryData.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2653">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2658">
   <si>
     <t>m1</t>
   </si>
@@ -8074,6 +8074,21 @@
   </si>
   <si>
     <t>[0.02238832003927956,0.02962412000064651]</t>
+  </si>
+  <si>
+    <t>[-1.3708705914009817e-11,5.909109089988267e-9]</t>
+  </si>
+  <si>
+    <t>[[0.0,0.0,1087.630668491096],[0.0,0.0,1087.6306699948068]]</t>
+  </si>
+  <si>
+    <t>[-133.44450336745595,-127.44908653846147]</t>
+  </si>
+  <si>
+    <t>[-55.227937499999996,-53.77970070615472]</t>
+  </si>
+  <si>
+    <t>[0.011788346425285258,0.015489408681294921]</t>
   </si>
 </sst>
 </file>
@@ -8491,7 +8506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE073501-CAF1-7547-9F20-DE970FECDDD2}">
-  <dimension ref="A1:W659"/>
+  <dimension ref="A1:W661"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
@@ -55298,6 +55313,148 @@
       </c>
       <c r="W659">
         <v>299365</v>
+      </c>
+    </row>
+    <row r="660" spans="1:23">
+      <c r="A660">
+        <v>1.5</v>
+      </c>
+      <c r="B660">
+        <v>1.5</v>
+      </c>
+      <c r="C660">
+        <v>1.0</v>
+      </c>
+      <c r="D660">
+        <v>26.0</v>
+      </c>
+      <c r="E660">
+        <v>0.0</v>
+      </c>
+      <c r="F660">
+        <v>80.0</v>
+      </c>
+      <c r="G660">
+        <v>0.0</v>
+      </c>
+      <c r="H660">
+        <v>0.0</v>
+      </c>
+      <c r="I660">
+        <v>0.0</v>
+      </c>
+      <c r="J660" t="s">
+        <v>1431</v>
+      </c>
+      <c r="K660">
+        <v>0.01</v>
+      </c>
+      <c r="L660" t="s">
+        <v>2653</v>
+      </c>
+      <c r="M660" t="s">
+        <v>2654</v>
+      </c>
+      <c r="N660" t="s">
+        <v>2655</v>
+      </c>
+      <c r="O660" t="s">
+        <v>2656</v>
+      </c>
+      <c r="P660" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q660" t="s">
+        <v>36</v>
+      </c>
+      <c r="R660">
+        <v>11.616999864578247</v>
+      </c>
+      <c r="S660" t="s">
+        <v>2657</v>
+      </c>
+      <c r="T660">
+        <v>1</v>
+      </c>
+      <c r="U660">
+        <v>660</v>
+      </c>
+      <c r="V660">
+        <v>1</v>
+      </c>
+      <c r="W660">
+        <v>302142</v>
+      </c>
+    </row>
+    <row r="661" spans="1:23">
+      <c r="A661">
+        <v>1.5</v>
+      </c>
+      <c r="B661">
+        <v>1.5</v>
+      </c>
+      <c r="C661">
+        <v>1.0</v>
+      </c>
+      <c r="D661">
+        <v>26.0</v>
+      </c>
+      <c r="E661">
+        <v>0.0</v>
+      </c>
+      <c r="F661">
+        <v>80.0</v>
+      </c>
+      <c r="G661">
+        <v>0.0</v>
+      </c>
+      <c r="H661">
+        <v>0.0</v>
+      </c>
+      <c r="I661">
+        <v>0.0</v>
+      </c>
+      <c r="J661" t="s">
+        <v>1431</v>
+      </c>
+      <c r="K661">
+        <v>0.01</v>
+      </c>
+      <c r="L661" t="s">
+        <v>2653</v>
+      </c>
+      <c r="M661" t="s">
+        <v>2654</v>
+      </c>
+      <c r="N661" t="s">
+        <v>2655</v>
+      </c>
+      <c r="O661" t="s">
+        <v>2656</v>
+      </c>
+      <c r="P661" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q661" t="s">
+        <v>36</v>
+      </c>
+      <c r="R661">
+        <v>7.50600004196167</v>
+      </c>
+      <c r="S661" t="s">
+        <v>2657</v>
+      </c>
+      <c r="T661">
+        <v>1</v>
+      </c>
+      <c r="U661">
+        <v>661</v>
+      </c>
+      <c r="V661">
+        <v>1</v>
+      </c>
+      <c r="W661">
+        <v>302142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>